<commit_message>
calibrate elec sector using guaranteed dispatch
</commit_message>
<xml_diff>
--- a/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
+++ b/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/users/nathaniyer/library/containers/com.microsoft.excel/data/state-eps-data-repository/template_state/elec/bgdpbes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\Alabama\AL-EPS\InputData\elec\BGDPbES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094B831B-97A2-1F47-B0E7-C814EF427FC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B895C02-D885-4B9F-AF84-803C89393441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="460" windowWidth="23000" windowHeight="11060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7785" yWindow="615" windowWidth="17880" windowHeight="16845" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -503,11 +503,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -515,42 +515,42 @@
         <v>44307</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -568,15 +568,17 @@
   </sheetPr>
   <dimension ref="A1:AK17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:37" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -689,7 +691,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -713,8 +715,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="H2">
         <f t="shared" si="0"/>
@@ -837,7 +838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -985,7 +986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1133,7 +1134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1281,7 +1282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1429,7 +1430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1577,7 +1578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1725,7 +1726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1873,7 +1874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -2021,7 +2022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -2169,7 +2170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -2317,7 +2318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -2465,7 +2466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -2613,7 +2614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -2726,7 +2727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -2839,7 +2840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>

</xml_diff>